<commit_message>
fix: minor improvements after discussion with Marten
</commit_message>
<xml_diff>
--- a/Mappings/HelpFromOthers - STU3.xlsx
+++ b/Mappings/HelpFromOthers - STU3.xlsx
@@ -275,7 +275,7 @@
     <t>CarePlan.activity.detail.category</t>
   </si>
   <si>
-    <t>CarePlan.note</t>
+    <t>CarePlan.activity.detail.description</t>
   </si>
 </sst>
 </file>
@@ -781,7 +781,7 @@
   <dimension ref="B2:Q11"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="P12" sqref="P12"/>
+      <selection activeCell="P15" sqref="P15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>

</xml_diff>